<commit_message>
added - blog videos
</commit_message>
<xml_diff>
--- a/data/blog_gallery_videos_journal.xlsx
+++ b/data/blog_gallery_videos_journal.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Imágenes" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t xml:space="preserve">TITULO</t>
   </si>
@@ -76,6 +76,27 @@
   </si>
   <si>
     <t xml:space="preserve">PASEO-REFORMA-3.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IFRAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Componentes de un exitoso centro comercial | Planigrupo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;iframe width="990" height="743" src="https://www.youtube.com/embed/HIUrz8sKWgI" title="Componentes de un exitoso centro comercial | Planigrupo" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La tecnología que transforma los centros comerciales | Planigrupo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;iframe width="990" height="558" src="https://www.youtube.com/embed/vH4mAj65qFg" title="La tecnología que transforma los centros comerciales" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qué considerar al elegir una ubicación para su centro comercial | Planigrupo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;iframe width="990" height="743" src="https://www.youtube.com/embed/Fh_gyPJ-Ib4" title="Qué considerar al elegir una ubicación para su centro comercial | Planigrupo" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" allowfullscreen&gt;&lt;/iframe&gt;</t>
   </si>
 </sst>
 </file>
@@ -85,11 +106,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -111,6 +133,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -161,13 +190,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -295,85 +336,85 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -393,14 +434,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="94.42"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
fixed - gallery height
</commit_message>
<xml_diff>
--- a/data/blog_gallery_videos_journal.xlsx
+++ b/data/blog_gallery_videos_journal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Imágenes" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t xml:space="preserve">TITULO</t>
   </si>
@@ -97,6 +97,66 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;iframe width="990" height="743" src="https://www.youtube.com/embed/Fh_gyPJ-Ib4" title="Qué considerar al elegir una ubicación para su centro comercial | Planigrupo" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TÍTULO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESCRIPCIÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEXTO BOTÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planigrupo construirá siete nuevos centros comerciales en el país</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La desarrolladora, que debutó el 29 de junio en la Bolsa Mexicana de Valores, buscará construir siete nuevos proyectos en el interior del país.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://expansion.mx/empresas/2016/07/12/planigrupo-construira-siete-nuevos-centros-comerciales-en-el-pais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expansion.mx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planigrupo prevé invertir 3 mil mdp en los próximos tres años</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La empresa mexicana reportó que la inversión será para abrir entre ocho y 12 centros comerciales en el país.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.elfinanciero.com.mx/empresas/planigrupo-preve-invertir-mil-mdp-en-los-proximos-tres-anos/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Financiero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLANIGRUPO reporta crecimiento de doble dígito en EBITDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLANIGRUPO LATAM, S.A.B. de C.V. y subsidiarias (“PLANIGRUPO”) (BMV: PLANI), empresa desarrolladora, operadora y propietaria de centros comerciales…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.prnewswire.com/news-releases/planigrupo-reporta-crecimiento-de-doble-digito-en-ebitda-y-mantuvo-una-tasa-de-ocupacion-del-94--870179772.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PR Newswire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planigrupo, con la mira en Sudamérica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hemos construido 65 de los 600 centros comerciales que hay en México. La colocación en la BMV nos permitirá seguir creciendo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.eleconomista.com.mx/mercados/Planigrupo-con-la-mira-en-Sudamerica-20160712-0025.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Economista</t>
   </si>
 </sst>
 </file>
@@ -106,7 +166,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -141,8 +201,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +221,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF333333"/>
         <bgColor rgb="FF333300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF666666"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
   </fills>
@@ -190,7 +264,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -203,12 +277,20 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -220,6 +302,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666666"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -336,8 +478,8 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -436,14 +578,14 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="94.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="94.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -458,7 +600,7 @@
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -466,7 +608,7 @@
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -474,7 +616,7 @@
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -494,14 +636,91 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="53.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.68"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="51.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>